<commit_message>
Some bugs and performance issues fixed. Also some cosmetic changes and other small things.
</commit_message>
<xml_diff>
--- a/excel/empresas.xlsx
+++ b/excel/empresas.xlsx
@@ -433,534 +433,534 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="42" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="42" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ano</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Restaurantes Abertos</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Porcentagem das Empresas em Atividade</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Ano</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Empresas Abertas</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>410</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>48%</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>410</v>
-      </c>
-      <c r="D2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1949</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="n">
-        <v>1949</v>
-      </c>
-      <c r="D3" t="n">
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1952</v>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" t="n">
-        <v>1952</v>
-      </c>
-      <c r="D4" t="n">
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1955</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" t="n">
-        <v>1955</v>
-      </c>
-      <c r="D5" t="n">
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1957</v>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" t="n">
-        <v>1957</v>
-      </c>
-      <c r="D6" t="n">
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1964</v>
+      </c>
+      <c r="B7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" t="n">
-        <v>1964</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-    </row>
     <row r="8">
-      <c r="C8" t="n">
+      <c r="A8" t="n">
         <v>1965</v>
       </c>
-      <c r="D8" t="n">
+      <c r="B8" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="C9" t="n">
+      <c r="A9" t="n">
         <v>1966</v>
       </c>
-      <c r="D9" t="n">
+      <c r="B9" t="n">
         <v>963</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="n">
+      <c r="A10" t="n">
         <v>1967</v>
       </c>
-      <c r="D10" t="n">
+      <c r="B10" t="n">
         <v>193</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11" t="n">
+      <c r="A11" t="n">
         <v>1968</v>
       </c>
-      <c r="D11" t="n">
+      <c r="B11" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="n">
+      <c r="A12" t="n">
         <v>1969</v>
       </c>
-      <c r="D12" t="n">
+      <c r="B12" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="n">
+      <c r="A13" t="n">
         <v>1970</v>
       </c>
-      <c r="D13" t="n">
+      <c r="B13" t="n">
         <v>281</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" t="n">
+      <c r="A14" t="n">
         <v>1971</v>
       </c>
-      <c r="D14" t="n">
+      <c r="B14" t="n">
         <v>395</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="n">
+      <c r="A15" t="n">
         <v>1972</v>
       </c>
-      <c r="D15" t="n">
+      <c r="B15" t="n">
         <v>468</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="n">
+      <c r="A16" t="n">
         <v>1973</v>
       </c>
-      <c r="D16" t="n">
+      <c r="B16" t="n">
         <v>562</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="n">
+      <c r="A17" t="n">
         <v>1974</v>
       </c>
-      <c r="D17" t="n">
+      <c r="B17" t="n">
         <v>644</v>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="n">
+      <c r="A18" t="n">
         <v>1975</v>
       </c>
-      <c r="D18" t="n">
+      <c r="B18" t="n">
         <v>751</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" t="n">
+      <c r="A19" t="n">
         <v>1976</v>
       </c>
-      <c r="D19" t="n">
+      <c r="B19" t="n">
         <v>1122</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" t="n">
+      <c r="A20" t="n">
         <v>1977</v>
       </c>
-      <c r="D20" t="n">
+      <c r="B20" t="n">
         <v>2354</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" t="n">
+      <c r="A21" t="n">
         <v>1978</v>
       </c>
-      <c r="D21" t="n">
+      <c r="B21" t="n">
         <v>2287</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22" t="n">
+      <c r="A22" t="n">
         <v>1979</v>
       </c>
-      <c r="D22" t="n">
+      <c r="B22" t="n">
         <v>2474</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="n">
+      <c r="A23" t="n">
         <v>1980</v>
       </c>
-      <c r="D23" t="n">
+      <c r="B23" t="n">
         <v>2889</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" t="n">
+      <c r="A24" t="n">
         <v>1981</v>
       </c>
-      <c r="D24" t="n">
+      <c r="B24" t="n">
         <v>2841</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" t="n">
+      <c r="A25" t="n">
         <v>1982</v>
       </c>
-      <c r="D25" t="n">
+      <c r="B25" t="n">
         <v>3269</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26" t="n">
+      <c r="A26" t="n">
         <v>1983</v>
       </c>
-      <c r="D26" t="n">
+      <c r="B26" t="n">
         <v>3978</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" t="n">
+      <c r="A27" t="n">
         <v>1984</v>
       </c>
-      <c r="D27" t="n">
+      <c r="B27" t="n">
         <v>3688</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" t="n">
+      <c r="A28" t="n">
         <v>1985</v>
       </c>
-      <c r="D28" t="n">
+      <c r="B28" t="n">
         <v>3945</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" t="n">
+      <c r="A29" t="n">
         <v>1986</v>
       </c>
-      <c r="D29" t="n">
+      <c r="B29" t="n">
         <v>5482</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="n">
+      <c r="A30" t="n">
         <v>1987</v>
       </c>
-      <c r="D30" t="n">
+      <c r="B30" t="n">
         <v>4915</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" t="n">
+      <c r="A31" t="n">
         <v>1988</v>
       </c>
-      <c r="D31" t="n">
+      <c r="B31" t="n">
         <v>5008</v>
       </c>
     </row>
     <row r="32">
-      <c r="C32" t="n">
+      <c r="A32" t="n">
         <v>1989</v>
       </c>
-      <c r="D32" t="n">
+      <c r="B32" t="n">
         <v>5671</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" t="n">
+      <c r="A33" t="n">
         <v>1990</v>
       </c>
-      <c r="D33" t="n">
+      <c r="B33" t="n">
         <v>6235</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" t="n">
+      <c r="A34" t="n">
         <v>1991</v>
       </c>
-      <c r="D34" t="n">
+      <c r="B34" t="n">
         <v>6280</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" t="n">
+      <c r="A35" t="n">
         <v>1992</v>
       </c>
-      <c r="D35" t="n">
+      <c r="B35" t="n">
         <v>5129</v>
       </c>
     </row>
     <row r="36">
-      <c r="C36" t="n">
+      <c r="A36" t="n">
         <v>1993</v>
       </c>
-      <c r="D36" t="n">
+      <c r="B36" t="n">
         <v>4943</v>
       </c>
     </row>
     <row r="37">
-      <c r="C37" t="n">
+      <c r="A37" t="n">
         <v>1994</v>
       </c>
-      <c r="D37" t="n">
+      <c r="B37" t="n">
         <v>4621</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" t="n">
+      <c r="A38" t="n">
         <v>1995</v>
       </c>
-      <c r="D38" t="n">
+      <c r="B38" t="n">
         <v>4503</v>
       </c>
     </row>
     <row r="39">
-      <c r="C39" t="n">
+      <c r="A39" t="n">
         <v>1996</v>
       </c>
-      <c r="D39" t="n">
+      <c r="B39" t="n">
         <v>4227</v>
       </c>
     </row>
     <row r="40">
-      <c r="C40" t="n">
+      <c r="A40" t="n">
         <v>1997</v>
       </c>
-      <c r="D40" t="n">
+      <c r="B40" t="n">
         <v>4243</v>
       </c>
     </row>
     <row r="41">
-      <c r="C41" t="n">
+      <c r="A41" t="n">
         <v>1998</v>
       </c>
-      <c r="D41" t="n">
+      <c r="B41" t="n">
         <v>3705</v>
       </c>
     </row>
     <row r="42">
-      <c r="C42" t="n">
+      <c r="A42" t="n">
         <v>1999</v>
       </c>
-      <c r="D42" t="n">
+      <c r="B42" t="n">
         <v>3578</v>
       </c>
     </row>
     <row r="43">
-      <c r="C43" t="n">
+      <c r="A43" t="n">
         <v>2000</v>
       </c>
-      <c r="D43" t="n">
+      <c r="B43" t="n">
         <v>3232</v>
       </c>
     </row>
     <row r="44">
-      <c r="C44" t="n">
+      <c r="A44" t="n">
         <v>2001</v>
       </c>
-      <c r="D44" t="n">
+      <c r="B44" t="n">
         <v>3442</v>
       </c>
     </row>
     <row r="45">
-      <c r="C45" t="n">
+      <c r="A45" t="n">
         <v>2002</v>
       </c>
-      <c r="D45" t="n">
+      <c r="B45" t="n">
         <v>3232</v>
       </c>
     </row>
     <row r="46">
-      <c r="C46" t="n">
+      <c r="A46" t="n">
         <v>2003</v>
       </c>
-      <c r="D46" t="n">
+      <c r="B46" t="n">
         <v>3109</v>
       </c>
     </row>
     <row r="47">
-      <c r="C47" t="n">
+      <c r="A47" t="n">
         <v>2004</v>
       </c>
-      <c r="D47" t="n">
+      <c r="B47" t="n">
         <v>2977</v>
       </c>
     </row>
     <row r="48">
-      <c r="C48" t="n">
+      <c r="A48" t="n">
         <v>2005</v>
       </c>
-      <c r="D48" t="n">
+      <c r="B48" t="n">
         <v>3432</v>
       </c>
     </row>
     <row r="49">
-      <c r="C49" t="n">
+      <c r="A49" t="n">
         <v>2006</v>
       </c>
-      <c r="D49" t="n">
+      <c r="B49" t="n">
         <v>3281</v>
       </c>
     </row>
     <row r="50">
-      <c r="C50" t="n">
+      <c r="A50" t="n">
         <v>2007</v>
       </c>
-      <c r="D50" t="n">
+      <c r="B50" t="n">
         <v>3750</v>
       </c>
     </row>
     <row r="51">
-      <c r="C51" t="n">
+      <c r="A51" t="n">
         <v>2008</v>
       </c>
-      <c r="D51" t="n">
+      <c r="B51" t="n">
         <v>4111</v>
       </c>
     </row>
     <row r="52">
-      <c r="C52" t="n">
+      <c r="A52" t="n">
         <v>2009</v>
       </c>
-      <c r="D52" t="n">
+      <c r="B52" t="n">
         <v>5428</v>
       </c>
     </row>
     <row r="53">
-      <c r="C53" t="n">
+      <c r="A53" t="n">
         <v>2010</v>
       </c>
-      <c r="D53" t="n">
+      <c r="B53" t="n">
         <v>10300</v>
       </c>
     </row>
     <row r="54">
-      <c r="C54" t="n">
+      <c r="A54" t="n">
         <v>2011</v>
       </c>
-      <c r="D54" t="n">
+      <c r="B54" t="n">
         <v>11120</v>
       </c>
     </row>
     <row r="55">
-      <c r="C55" t="n">
+      <c r="A55" t="n">
         <v>2012</v>
       </c>
-      <c r="D55" t="n">
+      <c r="B55" t="n">
         <v>11635</v>
       </c>
     </row>
     <row r="56">
-      <c r="C56" t="n">
+      <c r="A56" t="n">
         <v>2013</v>
       </c>
-      <c r="D56" t="n">
+      <c r="B56" t="n">
         <v>13793</v>
       </c>
     </row>
     <row r="57">
-      <c r="C57" t="n">
+      <c r="A57" t="n">
         <v>2014</v>
       </c>
-      <c r="D57" t="n">
+      <c r="B57" t="n">
         <v>14689</v>
       </c>
     </row>
     <row r="58">
-      <c r="C58" t="n">
+      <c r="A58" t="n">
         <v>2015</v>
       </c>
-      <c r="D58" t="n">
+      <c r="B58" t="n">
         <v>15651</v>
       </c>
     </row>
     <row r="59">
-      <c r="C59" t="n">
+      <c r="A59" t="n">
         <v>2016</v>
       </c>
-      <c r="D59" t="n">
+      <c r="B59" t="n">
         <v>16507</v>
       </c>
     </row>
     <row r="60">
-      <c r="C60" t="n">
+      <c r="A60" t="n">
         <v>2017</v>
       </c>
-      <c r="D60" t="n">
+      <c r="B60" t="n">
         <v>18882</v>
       </c>
     </row>
     <row r="61">
-      <c r="C61" t="n">
+      <c r="A61" t="n">
         <v>2018</v>
       </c>
-      <c r="D61" t="n">
+      <c r="B61" t="n">
         <v>34714</v>
       </c>
     </row>
     <row r="62">
-      <c r="C62" t="n">
+      <c r="A62" t="n">
         <v>2019</v>
       </c>
-      <c r="D62" t="n">
+      <c r="B62" t="n">
         <v>45585</v>
       </c>
     </row>
     <row r="63">
-      <c r="C63" t="n">
+      <c r="A63" t="n">
         <v>2020</v>
       </c>
-      <c r="D63" t="n">
+      <c r="B63" t="n">
         <v>50895</v>
       </c>
     </row>
     <row r="64">
-      <c r="C64" t="n">
+      <c r="A64" t="n">
         <v>2021</v>
       </c>
-      <c r="D64" t="n">
+      <c r="B64" t="n">
         <v>27348</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some files renamed. Added connection.py, which is a helper file that holds the database connection function. Important changes on writer.py and others
</commit_message>
<xml_diff>
--- a/excel/empresas.xlsx
+++ b/excel/empresas.xlsx
@@ -1,37 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anewe\PycharmProjects\Speedio-test\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9BD07-BE9D-42AD-AA60-0442371D1631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Restaurantes Abertos</t>
+  </si>
+  <si>
+    <t>Porcentagem das Empresas em Atividade</t>
+  </si>
+  <si>
+    <t>48%</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +69,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,551 +393,539 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="42" customWidth="1" min="4" max="4"/>
+    <col min="1" max="2" width="25" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ano</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Restaurantes Abertos</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Porcentagem das Empresas em Atividade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>410</v>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1941</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1949</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1952</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1955</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1957</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1964</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>1965</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>1966</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>963</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>1967</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>193</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>1968</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>236</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1969</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>303</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>1970</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>281</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>1971</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>395</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>1972</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>468</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1973</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>562</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1974</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>644</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>1975</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>751</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>1976</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>1122</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>1977</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>2354</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>1978</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>2287</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>1979</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>2474</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>1980</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>2889</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1981</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>2841</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1982</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>3269</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>1983</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>3978</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="n">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>1984</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>3688</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>1985</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>3945</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>1986</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>5482</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="n">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1987</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>4915</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>1988</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>5008</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>1989</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>5671</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>6235</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>1991</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>6280</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>1992</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>5129</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>1993</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>4943</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>1994</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>4621</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>1995</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>4503</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>1996</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>4227</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>1997</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>4243</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>1998</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>3705</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>1999</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>3578</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>2000</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>3232</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>2001</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>3442</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>2002</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>3232</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>2003</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>3109</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>2004</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>2977</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>2005</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>3432</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>2006</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>3281</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>2007</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>3750</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>2008</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>4111</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="n">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>2009</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>5428</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="n">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>2010</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>10300</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="n">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>2011</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>11120</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="n">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>2012</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>11635</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="n">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>2013</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>13793</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="n">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>2014</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>14689</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="n">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>2015</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>15651</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="n">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>2016</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>16507</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="n">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>2017</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>18882</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>2018</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>34714</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="n">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>2019</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>45585</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="n">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>2020</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>50895</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="n">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>2021</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>27348</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>